<commit_message>
FW test code for initial PCB HW test
</commit_message>
<xml_diff>
--- a/scripts/JY85-FW_Register_Map.xlsx
+++ b/scripts/JY85-FW_Register_Map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UBC_4TH_YEAR\ELEC-491\JY-85\project\JY85\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4DADAA-BEF6-40D2-89F8-4EDA3CFA8780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79B6D6C-8A04-47AF-A437-E1E82F59D8AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Register</t>
   </si>
@@ -69,6 +69,36 @@
   <si>
     <t>11-0: Sample_1
 23-12: Sample_2</t>
+  </si>
+  <si>
+    <t>23-0: Test_Current_Value</t>
+  </si>
+  <si>
+    <t>DVC_2PM_DCRESISTANCE_1</t>
+  </si>
+  <si>
+    <t>DVC_2PM_CURRVOLT_1</t>
+  </si>
+  <si>
+    <t>1-0: Sweep_Param</t>
+  </si>
+  <si>
+    <t>DVC_2PM_CURRVOLT_2</t>
+  </si>
+  <si>
+    <t>23-0: Starting_Param</t>
+  </si>
+  <si>
+    <t>DVC_2PM_CURRVOLT_3</t>
+  </si>
+  <si>
+    <t>DVC_2PM_CURRVOLT_4</t>
+  </si>
+  <si>
+    <t>23-0: Ending_Param</t>
+  </si>
+  <si>
+    <t>23-0: Increment_Param</t>
   </si>
   <si>
     <t>0: Start_Measure
@@ -352,10 +382,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G6" sqref="G6:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -403,7 +433,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -427,17 +457,92 @@
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2">
+        <v>5</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C10" s="3">
         <v>100</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test code for PCB driver circuits
</commit_message>
<xml_diff>
--- a/scripts/JY85-FW_Register_Map.xlsx
+++ b/scripts/JY85-FW_Register_Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UBC_4TH_YEAR\ELEC-491\JY-85\project\JY85\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79B6D6C-8A04-47AF-A437-E1E82F59D8AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABC9F98-AB38-4AF2-98B6-DE49F5742C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,9 +64,6 @@
 23-19: Probe_4_Config</t>
   </si>
   <si>
-    <t>DVC_SAMPLE_DATA</t>
-  </si>
-  <si>
     <t>11-0: Sample_1
 23-12: Sample_2</t>
   </si>
@@ -107,6 +104,9 @@
 3: Valid_Measure_Config
 5-4: Measure_Probe_Config
 9-6: Measure_Type_Config</t>
+  </si>
+  <si>
+    <t>DVC_FLUSH_SAMPLE_DATA</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G8"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -433,7 +433,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -459,10 +459,10 @@
     </row>
     <row r="5" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2">
         <v>3</v>
@@ -474,10 +474,10 @@
     </row>
     <row r="6" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="C6" s="2">
         <v>4</v>
@@ -489,10 +489,10 @@
     </row>
     <row r="7" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="C7" s="2">
         <v>5</v>
@@ -504,10 +504,10 @@
     </row>
     <row r="8" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="2">
         <v>6</v>
@@ -519,10 +519,10 @@
     </row>
     <row r="9" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2">
         <v>7</v>
@@ -534,10 +534,10 @@
     </row>
     <row r="10" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="C10" s="3">
         <v>100</v>

</xml_diff>

<commit_message>
new reg map, updated 2 measurements
</commit_message>
<xml_diff>
--- a/scripts/JY85-FW_Register_Map.xlsx
+++ b/scripts/JY85-FW_Register_Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\CAPSTONE\JY85\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778DF696-D935-4FAA-AAE2-B651A82B2585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5600877F-8916-45CB-B1D1-19DB2F3A501A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="71">
   <si>
     <t>Register</t>
   </si>
@@ -224,12 +224,34 @@
   <si>
     <t>DVC_2PM_LOWRESISTANCE_1</t>
   </si>
+  <si>
+    <t>DVC_3PM_TRANSCHAR_4</t>
+  </si>
+  <si>
+    <t>DVC_3PM_TRANSCHAR_5</t>
+  </si>
+  <si>
+    <t>DVC_3PM_OUTCHAR_4</t>
+  </si>
+  <si>
+    <t>DVC_3PM_OUTCHAR_5</t>
+  </si>
+  <si>
+    <t>23-0: Drain_Volt</t>
+  </si>
+  <si>
+    <t>23-0: Gate_Volt</t>
+  </si>
+  <si>
+    <t>23-0: Gate_Probe
+23-0: Drain_Probe</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -246,6 +268,11 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -498,10 +525,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -768,12 +795,12 @@
       </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="25" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="C18" s="2">
         <v>16</v>
@@ -788,7 +815,7 @@
         <v>44</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="C19" s="2">
         <v>17</v>
@@ -803,7 +830,7 @@
         <v>45</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C20" s="2">
         <v>18</v>
@@ -815,10 +842,10 @@
     </row>
     <row r="21" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C21" s="2">
         <v>19</v>
@@ -830,10 +857,10 @@
     </row>
     <row r="22" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C22" s="2">
         <v>20</v>
@@ -843,12 +870,12 @@
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="25" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="C23" s="2">
         <v>21</v>
@@ -860,10 +887,10 @@
     </row>
     <row r="24" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="C24" s="2">
         <v>22</v>
@@ -875,10 +902,10 @@
     </row>
     <row r="25" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="2">
         <v>23</v>
@@ -890,10 +917,10 @@
     </row>
     <row r="26" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" s="2">
         <v>24</v>
@@ -905,10 +932,10 @@
     </row>
     <row r="27" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C27" s="2">
         <v>25</v>
@@ -920,10 +947,10 @@
     </row>
     <row r="28" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C28" s="2">
         <v>26</v>
@@ -935,10 +962,10 @@
     </row>
     <row r="29" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C29" s="2">
         <v>27</v>
@@ -950,10 +977,10 @@
     </row>
     <row r="30" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C30" s="2">
         <v>28</v>
@@ -965,10 +992,10 @@
     </row>
     <row r="31" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C31" s="2">
         <v>29</v>
@@ -980,10 +1007,10 @@
     </row>
     <row r="32" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="C32" s="2">
         <v>30</v>
@@ -995,10 +1022,10 @@
     </row>
     <row r="33" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="C33" s="2">
         <v>31</v>
@@ -1010,10 +1037,10 @@
     </row>
     <row r="34" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C34" s="2">
         <v>32</v>
@@ -1025,10 +1052,10 @@
     </row>
     <row r="35" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C35" s="2">
         <v>33</v>
@@ -1040,10 +1067,10 @@
     </row>
     <row r="36" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="C36" s="2">
         <v>34</v>
@@ -1055,10 +1082,10 @@
     </row>
     <row r="37" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="C37" s="2">
         <v>35</v>
@@ -1070,10 +1097,10 @@
     </row>
     <row r="38" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C38" s="2">
         <v>36</v>
@@ -1085,47 +1112,108 @@
     </row>
     <row r="39" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="2">
+        <v>37</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="2">
+        <v>38</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" s="2">
+        <v>39</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" s="2">
+        <v>40</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B43" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C43" s="3">
         <v>100</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B44" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C44" s="2">
         <v>101</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D44" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C45" s="2">
         <v>102</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D45" s="3" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>